<commit_message>
FTLEE-1 Refactored Event class
</commit_message>
<xml_diff>
--- a/FTL Event XML.xlsx
+++ b/FTL Event XML.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="134">
   <si>
     <t>&lt;augment&gt;</t>
   </si>
@@ -324,9 +324,6 @@
     <t>They're trying to escape. TODO: Investigate further</t>
   </si>
   <si>
-    <t>Background images, TODO: Investigate</t>
-  </si>
-  <si>
     <t>&lt;item_modify&gt;
  &lt;item type="fuel" min="2" max="2"/&gt;
  &lt;item type="scrap" min="-2" max="4"/&gt;
@@ -406,9 +403,6 @@
   </si>
   <si>
     <t>&lt;boarders breach="true" min="1" max="8" class="human"/&gt;</t>
-  </si>
-  <si>
-    <t>load= textList TODO: Investigate hidden=, planet=, back=</t>
   </si>
   <si>
     <t>&lt;textList name="GAMEOVER"&gt;
@@ -453,6 +447,18 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>load= textList, planet=, back=</t>
+  </si>
+  <si>
+    <t>&lt;img back="BACKGROUND" planet="PLANET_POPULATED"/&gt;</t>
+  </si>
+  <si>
+    <t>Background images, loaded from lists</t>
+  </si>
+  <si>
+    <t>For &lt;img&gt;</t>
   </si>
 </sst>
 </file>
@@ -767,7 +773,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -778,33 +784,33 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
     <col min="3" max="3" width="72" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="63.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -816,9 +822,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -827,7 +833,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -838,7 +844,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -846,23 +855,26 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D7" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="8" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -873,47 +885,53 @@
         <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
       <c r="B9" t="s">
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
       <c r="B10" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -922,12 +940,12 @@
         <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -939,9 +957,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -950,63 +968,63 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
         <v>97</v>
       </c>
-      <c r="D18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -1017,18 +1035,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>5</v>
       </c>
@@ -1039,12 +1057,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>6</v>
       </c>
@@ -1055,51 +1073,51 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>14</v>
       </c>
@@ -1110,7 +1128,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>20</v>
       </c>
@@ -1118,19 +1136,19 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -1139,50 +1157,50 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
         <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B41" t="s">
         <v>25</v>
       </c>
       <c r="C41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
         <v>99</v>
       </c>
-      <c r="D41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
@@ -1194,50 +1212,50 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B45" t="s">
         <v>37</v>
       </c>
       <c r="C45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" t="s">
         <v>113</v>
       </c>
-      <c r="D45" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -1249,46 +1267,52 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>22</v>
       </c>
+      <c r="C49" t="s">
+        <v>131</v>
+      </c>
       <c r="D49" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>39</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D52" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1305,9 +1329,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
XML reference document updated - Thanks Kix!
</commit_message>
<xml_diff>
--- a/FTL Event XML.xlsx
+++ b/FTL Event XML.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="-24" windowWidth="20496" windowHeight="7776"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="140">
   <si>
     <t>&lt;augment&gt;</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>&lt;augment name="NANO_MEDBAY"/&gt;</t>
-  </si>
-  <si>
-    <t>RANDOM</t>
   </si>
   <si>
     <t>&lt;autoReward level="HIGH"&gt;scrap_only&lt;/autoReward&gt;</t>
@@ -159,9 +156,6 @@
 max_group="1" - the maximum possible "number" this option can apear as. Only for when there are two of the same option but one overrides the other, such as if you have a level 1 oxygen then you can pay 30 to upgrade but if you have level 2 then instead you have to pay 50</t>
   </si>
   <si>
-    <t>max&lt;9, class=race</t>
-  </si>
-  <si>
     <t>human</t>
   </si>
   <si>
@@ -227,10 +221,6 @@
   <si>
     <t>&lt;crewMember amount="1" all_skills="1" id="name_Charlie"/&gt;
 &lt;crewMember amount="-1" class="traitor"/&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class - race (or traitor)
-</t>
   </si>
   <si>
     <t>pilot="1"</t>
@@ -304,12 +294,6 @@
   </si>
   <si>
     <t>&lt;eventCounts sector="0"&gt;</t>
-  </si>
-  <si>
-    <t>TODO: Investigate</t>
-  </si>
-  <si>
-    <t>Lists events</t>
   </si>
   <si>
     <t>&lt;fleet&gt;rebel&lt;/fleet&gt;</t>
@@ -344,9 +328,6 @@
     <t>Negative delay, positive boost fleet</t>
   </si>
   <si>
-    <t>For weaponOverride</t>
-  </si>
-  <si>
     <t>steal="true" TODO - will take as much as it can up to the maximum determined (randomly generated betwen the two set numbers)</t>
   </si>
   <si>
@@ -372,13 +353,7 @@
 &lt;status type="clear" target="player/enemy" system="sensors" amount="100"/&gt;</t>
   </si>
   <si>
-    <t>type=clear, limit, divide, loss TODO: Investigate divide, loss. Add a status effect to a system. if using clear, the amount is in a percentage (100 being fully clear the system). effects do not stack on the same system</t>
-  </si>
-  <si>
     <t>Open a store. if this is declared outside of an &lt;event&gt; tag the beacon will show up as a store on the map</t>
-  </si>
-  <si>
-    <t>&lt;text id="event_ASTEROID_DERELICT_SHIP_SEARCH_3_c1_text"/&gt;</t>
   </si>
   <si>
     <t>&lt;unlockShip id="1"/&gt;</t>
@@ -414,9 +389,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>text and event only</t>
   </si>
   <si>
     <t>---</t>
@@ -460,13 +432,73 @@
   <si>
     <t>For &lt;img&gt;</t>
   </si>
+  <si>
+    <t>&lt;removeCrew&gt;</t>
+  </si>
+  <si>
+    <t>&lt;removeCrew class="engi"&gt;
+   &lt;clone&gt;true&lt;/clone&gt;
+   &lt;text id="event_ALISON_DEFECTOR_HELP_6_c0_clone"/&gt;
+&lt;/removeCrew&gt;</t>
+  </si>
+  <si>
+    <t>TODO: Investigate - Does it do anything?</t>
+  </si>
+  <si>
+    <t>See &lt;textList&gt;</t>
+  </si>
+  <si>
+    <t>List of events for &lt;event load=""&gt;</t>
+  </si>
+  <si>
+    <t>&lt;text id="event_ASTEROID_DERELICT_SHIP_SEARCH_3_c1_text"/&gt;
+&lt;text&gt;Your text directly here&lt;/text&gt;</t>
+  </si>
+  <si>
+    <t>List of texts for &lt;text load=""&gt;</t>
+  </si>
+  <si>
+    <t>Contains one text and one event only</t>
+  </si>
+  <si>
+    <t>Can also be RANDOM</t>
+  </si>
+  <si>
+    <t>Makes a quest marker that loads the event on that beacon</t>
+  </si>
+  <si>
+    <t>class=race (optional?)</t>
+  </si>
+  <si>
+    <t>type=clear, limit, divide, loss
+TODO: Investigate divide, loss. Add a status effect to a system. if using clear, the amount is in a percentage (100 being fully clear the system). effects do not stack on the same system</t>
+  </si>
+  <si>
+    <t>Class optional</t>
+  </si>
+  <si>
+    <t>class - race (or traitor)
+If you're removing crew it's better to use &lt;removeCrew&gt;
+amount can be negative if and only if class="traitor"</t>
+  </si>
+  <si>
+    <t>For weaponOverride TODO: Investigate - Used in Captain's Edition?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -494,13 +526,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,7 +806,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -781,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,43 +827,43 @@
     <col min="4" max="4" width="63.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" t="s">
-        <v>129</v>
+        <v>115</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -838,26 +871,38 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -865,87 +910,102 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
-        <v>111</v>
+      <c r="C9" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
+      </c>
+      <c r="D10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -954,23 +1014,23 @@
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
@@ -978,61 +1038,69 @@
     </row>
     <row r="17" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
         <v>95</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="2"/>
+      <c r="C20" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1040,26 +1108,35 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1067,252 +1144,317 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>116</v>
+      <c r="D28" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="34" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>20</v>
+      <c r="C34" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>122</v>
-      </c>
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" t="s">
-        <v>78</v>
+    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" t="s">
         <v>33</v>
       </c>
-      <c r="C39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" t="s">
-        <v>99</v>
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>77</v>
+      </c>
+      <c r="D43" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" t="s">
         <v>37</v>
       </c>
-      <c r="C45" t="s">
-        <v>112</v>
-      </c>
-      <c r="D45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>122</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" t="s">
         <v>19</v>
       </c>
-      <c r="C47" t="s">
-        <v>91</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" t="s">
-        <v>133</v>
+      <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>22</v>
       </c>
-      <c r="C49" t="s">
-        <v>131</v>
-      </c>
-      <c r="D49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" t="s">
-        <v>114</v>
+      <c r="C50" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
         <v>26</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>124</v>
+      <c r="B54" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1336,108 +1478,108 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>